<commit_message>
Added some metrics on the task
</commit_message>
<xml_diff>
--- a/BPMN-metrics-output.xlsx
+++ b/BPMN-metrics-output.xlsx
@@ -14,18 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>BPMN_File_Name</t>
   </si>
   <si>
-    <t>Start_Event</t>
-  </si>
-  <si>
-    <t>Process_element</t>
-  </si>
-  <si>
-    <t>Task_element</t>
+    <t>nTask</t>
+  </si>
+  <si>
+    <t>nSendTask</t>
+  </si>
+  <si>
+    <t>nUserTask</t>
+  </si>
+  <si>
+    <t>nManualTask</t>
+  </si>
+  <si>
+    <t>nBusinessRuleTask</t>
+  </si>
+  <si>
+    <t>nServiceTask</t>
+  </si>
+  <si>
+    <t>nScriptTask</t>
+  </si>
+  <si>
+    <t>nCallActivity</t>
+  </si>
+  <si>
+    <t>nSubProcess</t>
+  </si>
+  <si>
+    <t>nTransaction</t>
+  </si>
+  <si>
+    <t>nAdHocSubProcess</t>
   </si>
   <si>
     <t>test</t>
@@ -386,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,19 +429,67 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added metrics of group, participant, data object/store and gateways
</commit_message>
<xml_diff>
--- a/BPMN-metrics-output.xlsx
+++ b/BPMN-metrics-output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>BPMN_File_Name</t>
   </si>
@@ -50,6 +50,48 @@
   </si>
   <si>
     <t>nAdHocSubProcess</t>
+  </si>
+  <si>
+    <t>nGroup</t>
+  </si>
+  <si>
+    <t>nCollaboration</t>
+  </si>
+  <si>
+    <t>nLaneSet</t>
+  </si>
+  <si>
+    <t>nLane</t>
+  </si>
+  <si>
+    <t>nDataObject</t>
+  </si>
+  <si>
+    <t>nDataObjectReference</t>
+  </si>
+  <si>
+    <t>nDataStore</t>
+  </si>
+  <si>
+    <t>nDataStoreReference</t>
+  </si>
+  <si>
+    <t>nDataInput</t>
+  </si>
+  <si>
+    <t>nDataOutput</t>
+  </si>
+  <si>
+    <t>nExclusiveGateway</t>
+  </si>
+  <si>
+    <t>nParallelGateway</t>
+  </si>
+  <si>
+    <t>nInclusiveGateway</t>
+  </si>
+  <si>
+    <t>nEventBasedGateway</t>
   </si>
   <si>
     <t>test</t>
@@ -410,13 +452,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,10 +495,52 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -489,6 +573,48 @@
         <v>0</v>
       </c>
       <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented the start events group, all nested events are recognized but the main element e.g. endEvent/startEvent is considered
</commit_message>
<xml_diff>
--- a/BPMN-metrics-output.xlsx
+++ b/BPMN-metrics-output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>BPMN_File_Name</t>
   </si>
@@ -92,6 +92,39 @@
   </si>
   <si>
     <t>nEventBasedGateway</t>
+  </si>
+  <si>
+    <t>nCondition</t>
+  </si>
+  <si>
+    <t>nIntermediateThrowEvent</t>
+  </si>
+  <si>
+    <t>nStartEvent</t>
+  </si>
+  <si>
+    <t>nStartSignalEventDefinition</t>
+  </si>
+  <si>
+    <t>nStartConditionalEventDefinition</t>
+  </si>
+  <si>
+    <t>nStartTimerEventDefinition</t>
+  </si>
+  <si>
+    <t>nStartMessageEventDefinition</t>
+  </si>
+  <si>
+    <t>nStartCompensateEventDefinition</t>
+  </si>
+  <si>
+    <t>nStartCancelEventDefinition</t>
+  </si>
+  <si>
+    <t>nStartEscalationEventDefinition</t>
+  </si>
+  <si>
+    <t>nStartErrorEventDefinition</t>
   </si>
   <si>
     <t>test</t>
@@ -452,13 +485,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,10 +570,43 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -615,6 +681,39 @@
         <v>0</v>
       </c>
       <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
         <v>0</v>
       </c>
     </row>

</xml_diff>